<commit_message>
Fighter 2 bullets doubled.
</commit_message>
<xml_diff>
--- a/Artwork/Font.xlsx
+++ b/Artwork/Font.xlsx
@@ -1,39 +1,53 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonholmes/Documents/GitHub/Nineteen43/Artwork/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon.holmes\Documents\GitHub\Nineteen44\Artwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF615754-8EA4-4428-95E3-96CF2E6B8EF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11240" yWindow="17280" windowWidth="38160" windowHeight="13780" tabRatio="500"/>
+    <workbookView xWindow="11235" yWindow="17280" windowWidth="38160" windowHeight="13785" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2 (3)" sheetId="9" r:id="rId1"/>
+    <sheet name="Sheet2 (4)" sheetId="10" r:id="rId1"/>
+    <sheet name="Sheet2 (3)" sheetId="9" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="LDMAX" localSheetId="1">#REF!</definedName>
     <definedName name="LDMAX" localSheetId="0">#REF!</definedName>
     <definedName name="LDMAX">#REF!</definedName>
+    <definedName name="LDMIN" localSheetId="1">#REF!</definedName>
     <definedName name="LDMIN" localSheetId="0">#REF!</definedName>
     <definedName name="LDMIN">#REF!</definedName>
+    <definedName name="LS_HR_MAX" localSheetId="1">#REF!</definedName>
     <definedName name="LS_HR_MAX" localSheetId="0">#REF!</definedName>
     <definedName name="LS_HR_MAX">#REF!</definedName>
+    <definedName name="LS_HR_MIN" localSheetId="1">#REF!</definedName>
     <definedName name="LS_HR_MIN" localSheetId="0">#REF!</definedName>
     <definedName name="LS_HR_MIN">#REF!</definedName>
+    <definedName name="LS_LR_MAX" localSheetId="1">#REF!</definedName>
     <definedName name="LS_LR_MAX" localSheetId="0">#REF!</definedName>
     <definedName name="LS_LR_MAX">#REF!</definedName>
+    <definedName name="LS_LR_MIN" localSheetId="1">#REF!</definedName>
     <definedName name="LS_LR_MIN" localSheetId="0">#REF!</definedName>
     <definedName name="LS_LR_MIN">#REF!</definedName>
+    <definedName name="lSMIN" localSheetId="1">#REF!</definedName>
     <definedName name="lSMIN" localSheetId="0">#REF!</definedName>
     <definedName name="lSMIN">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -43,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="1">
   <si>
     <t>¢</t>
   </si>
@@ -51,8 +65,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -199,7 +213,7 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="9"/>
+    <cellStyle name="Normal 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -476,19 +490,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFA50DD6-CC5B-4EDA-BECC-6628D9367CB3}">
   <dimension ref="A1:FR10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="160" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="160" workbookViewId="0">
       <selection activeCell="BZ19" sqref="BZ19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="2.6640625" style="1"/>
+    <col min="1" max="16384" width="2.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:174">
+    <row r="1" spans="1:174" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="7">
@@ -996,7 +1010,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:174" ht="16">
+    <row r="2" spans="1:174" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1049,7 +1063,7 @@
       <c r="EY2" s="4"/>
       <c r="EZ2" s="4"/>
     </row>
-    <row r="3" spans="1:174" ht="16">
+    <row r="3" spans="1:174" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1244,7 +1258,7 @@
       <c r="FL3" s="4"/>
       <c r="FM3" s="4"/>
     </row>
-    <row r="4" spans="1:174" ht="16">
+    <row r="4" spans="1:174" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>4</v>
       </c>
@@ -1439,7 +1453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:174" ht="16">
+    <row r="5" spans="1:174" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>8</v>
       </c>
@@ -1643,7 +1657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:174" ht="16">
+    <row r="6" spans="1:174" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>16</v>
       </c>
@@ -1865,7 +1879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:174" ht="16">
+    <row r="7" spans="1:174" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>32</v>
       </c>
@@ -1960,7 +1974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:174" ht="16">
+    <row r="8" spans="1:174" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>64</v>
       </c>
@@ -2044,7 +2058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:174" ht="16">
+    <row r="9" spans="1:174" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>128</v>
       </c>
@@ -2122,7 +2136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:174">
+    <row r="10" spans="1:174" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="2" t="str">
@@ -2638,7 +2652,7 @@
         <v>0x00,</v>
       </c>
       <c r="EA10" s="2" t="str">
-        <f t="shared" ref="EA10:EL10" si="2">"0x"&amp;DEC2HEX((SUMIF(EA$2:EA$9,"&lt;&gt;",$A$2:$A$9)),2)&amp;","</f>
+        <f t="shared" ref="EA10:ET10" si="2">"0x"&amp;DEC2HEX((SUMIF(EA$2:EA$9,"&lt;&gt;",$A$2:$A$9)),2)&amp;","</f>
         <v>0x00,</v>
       </c>
       <c r="EB10" s="2" t="str">
@@ -2686,121 +2700,121 @@
         <v>0x00,</v>
       </c>
       <c r="EM10" s="2" t="str">
-        <f t="shared" ref="ED10:ET10" si="3">"0x"&amp;DEC2HEX((SUMIF(EM$2:EM$9,"&lt;&gt;",$A$2:$A$9)),2)&amp;","</f>
+        <f t="shared" si="2"/>
         <v>0xFE,</v>
       </c>
       <c r="EN10" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFE,</v>
+      </c>
+      <c r="EO10" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFE,</v>
+      </c>
+      <c r="EP10" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFC,</v>
+      </c>
+      <c r="EQ10" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFC,</v>
+      </c>
+      <c r="ER10" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>0xF8,</v>
+      </c>
+      <c r="ES10" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>0xF0,</v>
+      </c>
+      <c r="ET10" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>0xC0,</v>
+      </c>
+      <c r="EW10" s="2" t="str">
+        <f t="shared" ref="EW10:FH10" si="3">"0x"&amp;DEC2HEX((SUMIF(EW$2:EW$9,"&lt;&gt;",$A$2:$A$9)),2)&amp;","</f>
+        <v>0x70,</v>
+      </c>
+      <c r="EX10" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x00,</v>
+      </c>
+      <c r="EY10" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>0xF8,</v>
+      </c>
+      <c r="EZ10" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x00,</v>
+      </c>
+      <c r="FA10" s="2" t="str">
         <f t="shared" si="3"/>
         <v>0xFE,</v>
       </c>
-      <c r="EO10" s="2" t="str">
+      <c r="FB10" s="2" t="str">
         <f t="shared" si="3"/>
         <v>0xFE,</v>
       </c>
-      <c r="EP10" s="2" t="str">
+      <c r="FC10" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>0xFE,</v>
+      </c>
+      <c r="FD10" s="2" t="str">
         <f t="shared" si="3"/>
         <v>0xFC,</v>
       </c>
-      <c r="EQ10" s="2" t="str">
+      <c r="FE10" s="2" t="str">
         <f t="shared" si="3"/>
         <v>0xFC,</v>
       </c>
-      <c r="ER10" s="2" t="str">
+      <c r="FF10" s="2" t="str">
         <f t="shared" si="3"/>
         <v>0xF8,</v>
       </c>
-      <c r="ES10" s="2" t="str">
+      <c r="FG10" s="2" t="str">
         <f t="shared" si="3"/>
         <v>0xF0,</v>
       </c>
-      <c r="ET10" s="2" t="str">
+      <c r="FH10" s="2" t="str">
         <f t="shared" si="3"/>
         <v>0xC0,</v>
       </c>
-      <c r="EW10" s="2" t="str">
-        <f t="shared" ref="EW10:FH10" si="4">"0x"&amp;DEC2HEX((SUMIF(EW$2:EW$9,"&lt;&gt;",$A$2:$A$9)),2)&amp;","</f>
+      <c r="FK10" s="2" t="str">
+        <f t="shared" ref="FK10:FR10" si="4">"0x"&amp;DEC2HEX((SUMIF(FK$2:FK$9,"&lt;&gt;",$A$2:$A$9)),2)&amp;","</f>
         <v>0x70,</v>
       </c>
-      <c r="EX10" s="2" t="str">
+      <c r="FL10" s="2" t="str">
         <f t="shared" si="4"/>
         <v>0x00,</v>
       </c>
-      <c r="EY10" s="2" t="str">
+      <c r="FM10" s="2" t="str">
         <f t="shared" si="4"/>
         <v>0xF8,</v>
       </c>
-      <c r="EZ10" s="2" t="str">
+      <c r="FN10" s="2" t="str">
         <f t="shared" si="4"/>
         <v>0x00,</v>
       </c>
-      <c r="FA10" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>0xFE,</v>
-      </c>
-      <c r="FB10" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>0xFE,</v>
-      </c>
-      <c r="FC10" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>0xFE,</v>
-      </c>
-      <c r="FD10" s="2" t="str">
+      <c r="FO10" s="2" t="str">
         <f t="shared" si="4"/>
         <v>0xFC,</v>
       </c>
-      <c r="FE10" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>0xFC,</v>
-      </c>
-      <c r="FF10" s="2" t="str">
+      <c r="FP10" s="2" t="str">
         <f t="shared" si="4"/>
         <v>0xF8,</v>
       </c>
-      <c r="FG10" s="2" t="str">
+      <c r="FQ10" s="2" t="str">
         <f t="shared" si="4"/>
         <v>0xF0,</v>
       </c>
-      <c r="FH10" s="2" t="str">
+      <c r="FR10" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>0xC0,</v>
-      </c>
-      <c r="FK10" s="2" t="str">
-        <f t="shared" ref="FK10:FR10" si="5">"0x"&amp;DEC2HEX((SUMIF(FK$2:FK$9,"&lt;&gt;",$A$2:$A$9)),2)&amp;","</f>
-        <v>0x70,</v>
-      </c>
-      <c r="FL10" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>0x00,</v>
-      </c>
-      <c r="FM10" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>0xF8,</v>
-      </c>
-      <c r="FN10" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>0x00,</v>
-      </c>
-      <c r="FO10" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>0xFC,</v>
-      </c>
-      <c r="FP10" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>0xF8,</v>
-      </c>
-      <c r="FQ10" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>0xF0,</v>
-      </c>
-      <c r="FR10" s="2" t="str">
-        <f t="shared" si="5"/>
         <v>0xC0,</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="EW2:EZ2 FK4:FM4 EW3:EY9 FK5:FL9">
-    <cfRule type="colorScale" priority="8237">
+    <cfRule type="colorScale" priority="279">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2810,7 +2824,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="colorScale" priority="1361">
+    <cfRule type="colorScale" priority="278">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2820,7 +2834,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="colorScale" priority="1360">
+    <cfRule type="colorScale" priority="277">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2830,7 +2844,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="colorScale" priority="1353">
+    <cfRule type="colorScale" priority="276">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2840,7 +2854,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="colorScale" priority="1321">
+    <cfRule type="colorScale" priority="275">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2850,7 +2864,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="colorScale" priority="1317">
+    <cfRule type="colorScale" priority="274">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2860,7 +2874,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8:F9">
-    <cfRule type="colorScale" priority="1316">
+    <cfRule type="colorScale" priority="273">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2870,7 +2884,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:J9">
-    <cfRule type="colorScale" priority="1315">
+    <cfRule type="colorScale" priority="272">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2880,7 +2894,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7:L7 K8:O9">
-    <cfRule type="colorScale" priority="1313">
+    <cfRule type="colorScale" priority="271">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2890,7 +2904,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7:O7">
-    <cfRule type="colorScale" priority="1312">
+    <cfRule type="colorScale" priority="270">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2900,7 +2914,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P9:AF9 P7:AD8">
-    <cfRule type="colorScale" priority="1311">
+    <cfRule type="colorScale" priority="269">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2910,7 +2924,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EM3:EO3">
-    <cfRule type="colorScale" priority="773">
+    <cfRule type="colorScale" priority="268">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2920,7 +2934,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EP4:EQ4">
-    <cfRule type="colorScale" priority="772">
+    <cfRule type="colorScale" priority="267">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2930,7 +2944,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="ER5">
-    <cfRule type="colorScale" priority="771">
+    <cfRule type="colorScale" priority="266">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2940,7 +2954,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="ES6:ES7">
-    <cfRule type="colorScale" priority="770">
+    <cfRule type="colorScale" priority="265">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2950,7 +2964,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="ET8:ET9">
-    <cfRule type="colorScale" priority="769">
+    <cfRule type="colorScale" priority="264">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2960,7 +2974,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="ES8:ES9">
-    <cfRule type="colorScale" priority="750">
+    <cfRule type="colorScale" priority="263">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2970,7 +2984,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EM5:EQ5">
-    <cfRule type="colorScale" priority="749">
+    <cfRule type="colorScale" priority="262">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2980,7 +2994,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EM4:EO4">
-    <cfRule type="colorScale" priority="748">
+    <cfRule type="colorScale" priority="261">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2990,7 +3004,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="ES8:ES9">
-    <cfRule type="colorScale" priority="746">
+    <cfRule type="colorScale" priority="260">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3000,7 +3014,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EM4">
-    <cfRule type="colorScale" priority="742">
+    <cfRule type="colorScale" priority="259">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3010,7 +3024,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EM5">
-    <cfRule type="colorScale" priority="741">
+    <cfRule type="colorScale" priority="258">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3020,7 +3034,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EM6:ER9">
-    <cfRule type="colorScale" priority="737">
+    <cfRule type="colorScale" priority="257">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3030,7 +3044,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FA3:FC3">
-    <cfRule type="colorScale" priority="593">
+    <cfRule type="colorScale" priority="256">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3040,7 +3054,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FD4:FE4">
-    <cfRule type="colorScale" priority="592">
+    <cfRule type="colorScale" priority="255">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3050,7 +3064,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FF5">
-    <cfRule type="colorScale" priority="591">
+    <cfRule type="colorScale" priority="254">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3060,7 +3074,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FG6:FG7">
-    <cfRule type="colorScale" priority="590">
+    <cfRule type="colorScale" priority="253">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3070,7 +3084,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FH8:FH9">
-    <cfRule type="colorScale" priority="589">
+    <cfRule type="colorScale" priority="252">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3080,7 +3094,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FG8:FG9">
-    <cfRule type="colorScale" priority="570">
+    <cfRule type="colorScale" priority="251">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3090,7 +3104,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EZ5:FE5">
-    <cfRule type="colorScale" priority="569">
+    <cfRule type="colorScale" priority="250">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3100,7 +3114,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EZ4:FC4">
-    <cfRule type="colorScale" priority="568">
+    <cfRule type="colorScale" priority="249">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3110,7 +3124,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EZ3">
-    <cfRule type="colorScale" priority="567">
+    <cfRule type="colorScale" priority="248">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3120,7 +3134,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FG8:FG9">
-    <cfRule type="colorScale" priority="566">
+    <cfRule type="colorScale" priority="247">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3130,7 +3144,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FA4">
-    <cfRule type="colorScale" priority="562">
+    <cfRule type="colorScale" priority="246">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3140,7 +3154,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EZ5:FA5">
-    <cfRule type="colorScale" priority="561">
+    <cfRule type="colorScale" priority="245">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3150,7 +3164,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EZ4">
-    <cfRule type="colorScale" priority="560">
+    <cfRule type="colorScale" priority="244">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3160,7 +3174,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EZ6:FF9">
-    <cfRule type="colorScale" priority="557">
+    <cfRule type="colorScale" priority="243">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3170,7 +3184,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FK3:FM3">
-    <cfRule type="colorScale" priority="409">
+    <cfRule type="colorScale" priority="242">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3180,7 +3194,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FN4:FO4">
-    <cfRule type="colorScale" priority="408">
+    <cfRule type="colorScale" priority="241">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3190,7 +3204,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FP5">
-    <cfRule type="colorScale" priority="407">
+    <cfRule type="colorScale" priority="240">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3200,7 +3214,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FQ6:FQ7">
-    <cfRule type="colorScale" priority="406">
+    <cfRule type="colorScale" priority="239">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3210,7 +3224,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FR8:FR9">
-    <cfRule type="colorScale" priority="405">
+    <cfRule type="colorScale" priority="238">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3220,7 +3234,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FQ8:FQ9">
-    <cfRule type="colorScale" priority="386">
+    <cfRule type="colorScale" priority="237">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3230,7 +3244,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FN5:FO5">
-    <cfRule type="colorScale" priority="385">
+    <cfRule type="colorScale" priority="236">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3240,7 +3254,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FQ8:FQ9">
-    <cfRule type="colorScale" priority="382">
+    <cfRule type="colorScale" priority="235">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3250,7 +3264,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FK4">
-    <cfRule type="colorScale" priority="378">
+    <cfRule type="colorScale" priority="234">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3260,7 +3274,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FN6:FP9">
-    <cfRule type="colorScale" priority="373">
+    <cfRule type="colorScale" priority="233">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3270,7 +3284,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FM5:FM9">
-    <cfRule type="colorScale" priority="239">
+    <cfRule type="colorScale" priority="232">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3280,7 +3294,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="colorScale" priority="238">
+    <cfRule type="colorScale" priority="231">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3290,7 +3304,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="colorScale" priority="237">
+    <cfRule type="colorScale" priority="230">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3300,7 +3314,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="colorScale" priority="236">
+    <cfRule type="colorScale" priority="229">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3310,7 +3324,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="colorScale" priority="235">
+    <cfRule type="colorScale" priority="228">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3320,7 +3334,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="colorScale" priority="234">
+    <cfRule type="colorScale" priority="227">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3330,7 +3344,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="colorScale" priority="233">
+    <cfRule type="colorScale" priority="226">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3340,7 +3354,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="colorScale" priority="232">
+    <cfRule type="colorScale" priority="225">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3350,7 +3364,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="colorScale" priority="231">
+    <cfRule type="colorScale" priority="224">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3360,7 +3374,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="colorScale" priority="230">
+    <cfRule type="colorScale" priority="223">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3370,7 +3384,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="colorScale" priority="229">
+    <cfRule type="colorScale" priority="222">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3380,7 +3394,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="colorScale" priority="228">
+    <cfRule type="colorScale" priority="221">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3390,7 +3404,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="colorScale" priority="227">
+    <cfRule type="colorScale" priority="220">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3400,7 +3414,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="colorScale" priority="226">
+    <cfRule type="colorScale" priority="219">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3410,7 +3424,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="colorScale" priority="225">
+    <cfRule type="colorScale" priority="218">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3420,7 +3434,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="colorScale" priority="223">
+    <cfRule type="colorScale" priority="217">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3430,7 +3444,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="colorScale" priority="222">
+    <cfRule type="colorScale" priority="216">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3440,7 +3454,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="colorScale" priority="221">
+    <cfRule type="colorScale" priority="215">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3450,7 +3464,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="colorScale" priority="220">
+    <cfRule type="colorScale" priority="214">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3460,7 +3474,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="colorScale" priority="219">
+    <cfRule type="colorScale" priority="213">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3470,7 +3484,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="colorScale" priority="218">
+    <cfRule type="colorScale" priority="212">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3480,7 +3494,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2">
-    <cfRule type="colorScale" priority="217">
+    <cfRule type="colorScale" priority="211">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3490,7 +3504,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3">
-    <cfRule type="colorScale" priority="216">
+    <cfRule type="colorScale" priority="210">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3500,7 +3514,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4">
-    <cfRule type="colorScale" priority="215">
+    <cfRule type="colorScale" priority="209">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3510,7 +3524,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="colorScale" priority="214">
+    <cfRule type="colorScale" priority="208">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3520,7 +3534,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="colorScale" priority="213">
+    <cfRule type="colorScale" priority="207">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3530,7 +3544,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6">
-    <cfRule type="colorScale" priority="212">
+    <cfRule type="colorScale" priority="206">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3540,7 +3554,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3">
-    <cfRule type="colorScale" priority="211">
+    <cfRule type="colorScale" priority="205">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3550,7 +3564,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4">
-    <cfRule type="colorScale" priority="210">
+    <cfRule type="colorScale" priority="204">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3560,7 +3574,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M5">
-    <cfRule type="colorScale" priority="209">
+    <cfRule type="colorScale" priority="203">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3570,7 +3584,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3">
-    <cfRule type="colorScale" priority="207">
+    <cfRule type="colorScale" priority="202">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3580,7 +3594,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4">
-    <cfRule type="colorScale" priority="206">
+    <cfRule type="colorScale" priority="201">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3590,7 +3604,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O5">
-    <cfRule type="colorScale" priority="205">
+    <cfRule type="colorScale" priority="200">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3600,7 +3614,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O6">
-    <cfRule type="colorScale" priority="204">
+    <cfRule type="colorScale" priority="199">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3610,7 +3624,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P6">
-    <cfRule type="colorScale" priority="203">
+    <cfRule type="colorScale" priority="198">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3620,7 +3634,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q6">
-    <cfRule type="colorScale" priority="202">
+    <cfRule type="colorScale" priority="197">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3630,7 +3644,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3">
-    <cfRule type="colorScale" priority="201">
+    <cfRule type="colorScale" priority="196">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3640,7 +3654,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3">
-    <cfRule type="colorScale" priority="200">
+    <cfRule type="colorScale" priority="195">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3650,7 +3664,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3">
-    <cfRule type="colorScale" priority="199">
+    <cfRule type="colorScale" priority="194">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3660,7 +3674,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U3">
-    <cfRule type="colorScale" priority="198">
+    <cfRule type="colorScale" priority="193">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3670,7 +3684,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2">
-    <cfRule type="colorScale" priority="197">
+    <cfRule type="colorScale" priority="192">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3680,7 +3694,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U4">
-    <cfRule type="colorScale" priority="196">
+    <cfRule type="colorScale" priority="191">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3690,7 +3704,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U5">
-    <cfRule type="colorScale" priority="195">
+    <cfRule type="colorScale" priority="190">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3700,7 +3714,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U6">
-    <cfRule type="colorScale" priority="194">
+    <cfRule type="colorScale" priority="189">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3710,7 +3724,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T6">
-    <cfRule type="colorScale" priority="193">
+    <cfRule type="colorScale" priority="188">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3720,7 +3734,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S5">
-    <cfRule type="colorScale" priority="192">
+    <cfRule type="colorScale" priority="187">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3730,7 +3744,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S4">
-    <cfRule type="colorScale" priority="191">
+    <cfRule type="colorScale" priority="186">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3740,7 +3754,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X3">
-    <cfRule type="colorScale" priority="190">
+    <cfRule type="colorScale" priority="185">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3750,7 +3764,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W4">
-    <cfRule type="colorScale" priority="189">
+    <cfRule type="colorScale" priority="184">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3760,7 +3774,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y4">
-    <cfRule type="colorScale" priority="188">
+    <cfRule type="colorScale" priority="183">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3770,7 +3784,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W5">
-    <cfRule type="colorScale" priority="187">
+    <cfRule type="colorScale" priority="182">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3780,7 +3794,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X5">
-    <cfRule type="colorScale" priority="186">
+    <cfRule type="colorScale" priority="181">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3790,7 +3804,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X6">
-    <cfRule type="colorScale" priority="185">
+    <cfRule type="colorScale" priority="180">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3800,7 +3814,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y6">
-    <cfRule type="colorScale" priority="184">
+    <cfRule type="colorScale" priority="179">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3810,7 +3824,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2">
-    <cfRule type="colorScale" priority="183">
+    <cfRule type="colorScale" priority="178">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3820,7 +3834,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2">
-    <cfRule type="colorScale" priority="182">
+    <cfRule type="colorScale" priority="177">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3830,7 +3844,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC4">
-    <cfRule type="colorScale" priority="181">
+    <cfRule type="colorScale" priority="176">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3840,7 +3854,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB4">
-    <cfRule type="colorScale" priority="180">
+    <cfRule type="colorScale" priority="175">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3850,7 +3864,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA4">
-    <cfRule type="colorScale" priority="179">
+    <cfRule type="colorScale" priority="174">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3860,7 +3874,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB3">
-    <cfRule type="colorScale" priority="178">
+    <cfRule type="colorScale" priority="173">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3870,7 +3884,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB5">
-    <cfRule type="colorScale" priority="177">
+    <cfRule type="colorScale" priority="172">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3880,7 +3894,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB6">
-    <cfRule type="colorScale" priority="176">
+    <cfRule type="colorScale" priority="171">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3890,7 +3904,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG8:EL9 AH7:AO7 AQ7:BM7 BO7:BS7 BU7:CW7 CZ7:EL7">
-    <cfRule type="colorScale" priority="175">
+    <cfRule type="colorScale" priority="170">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3900,7 +3914,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE3">
-    <cfRule type="colorScale" priority="174">
+    <cfRule type="colorScale" priority="169">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3910,7 +3924,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF3">
-    <cfRule type="colorScale" priority="173">
+    <cfRule type="colorScale" priority="168">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3920,7 +3934,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG3">
-    <cfRule type="colorScale" priority="172">
+    <cfRule type="colorScale" priority="167">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3930,7 +3944,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE4">
-    <cfRule type="colorScale" priority="171">
+    <cfRule type="colorScale" priority="166">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3940,7 +3954,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE5">
-    <cfRule type="colorScale" priority="170">
+    <cfRule type="colorScale" priority="165">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3950,7 +3964,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG5">
-    <cfRule type="colorScale" priority="168">
+    <cfRule type="colorScale" priority="164">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3960,7 +3974,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG4">
-    <cfRule type="colorScale" priority="167">
+    <cfRule type="colorScale" priority="163">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3970,7 +3984,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG6">
-    <cfRule type="colorScale" priority="166">
+    <cfRule type="colorScale" priority="162">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3980,7 +3994,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE8">
-    <cfRule type="colorScale" priority="163">
+    <cfRule type="colorScale" priority="161">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3990,7 +4004,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF8">
-    <cfRule type="colorScale" priority="162">
+    <cfRule type="colorScale" priority="160">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4000,7 +4014,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG7">
-    <cfRule type="colorScale" priority="161">
+    <cfRule type="colorScale" priority="159">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4010,7 +4024,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF6">
-    <cfRule type="colorScale" priority="160">
+    <cfRule type="colorScale" priority="158">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4020,7 +4034,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE6">
-    <cfRule type="colorScale" priority="159">
+    <cfRule type="colorScale" priority="157">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4030,7 +4044,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF5">
-    <cfRule type="colorScale" priority="158">
+    <cfRule type="colorScale" priority="156">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4040,7 +4054,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF7">
-    <cfRule type="colorScale" priority="157">
+    <cfRule type="colorScale" priority="155">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4050,7 +4064,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE7">
-    <cfRule type="colorScale" priority="156">
+    <cfRule type="colorScale" priority="154">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4060,7 +4074,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI2">
-    <cfRule type="colorScale" priority="155">
+    <cfRule type="colorScale" priority="153">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4070,7 +4084,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI3">
-    <cfRule type="colorScale" priority="154">
+    <cfRule type="colorScale" priority="152">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4080,7 +4094,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI4">
-    <cfRule type="colorScale" priority="153">
+    <cfRule type="colorScale" priority="151">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4090,7 +4104,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI5">
-    <cfRule type="colorScale" priority="152">
+    <cfRule type="colorScale" priority="150">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4100,7 +4114,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI6">
-    <cfRule type="colorScale" priority="151">
+    <cfRule type="colorScale" priority="149">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4110,7 +4124,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ3">
-    <cfRule type="colorScale" priority="150">
+    <cfRule type="colorScale" priority="148">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4120,7 +4134,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK4">
-    <cfRule type="colorScale" priority="149">
+    <cfRule type="colorScale" priority="147">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4130,7 +4144,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK5">
-    <cfRule type="colorScale" priority="148">
+    <cfRule type="colorScale" priority="146">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4140,7 +4154,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK6">
-    <cfRule type="colorScale" priority="147">
+    <cfRule type="colorScale" priority="145">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4150,7 +4164,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN6">
-    <cfRule type="colorScale" priority="146">
+    <cfRule type="colorScale" priority="144">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4160,7 +4174,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN5">
-    <cfRule type="colorScale" priority="145">
+    <cfRule type="colorScale" priority="143">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4170,7 +4184,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN4">
-    <cfRule type="colorScale" priority="144">
+    <cfRule type="colorScale" priority="142">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4180,7 +4194,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN2">
-    <cfRule type="colorScale" priority="143">
+    <cfRule type="colorScale" priority="141">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4190,7 +4204,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ4">
-    <cfRule type="colorScale" priority="142">
+    <cfRule type="colorScale" priority="140">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4200,7 +4214,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ5">
-    <cfRule type="colorScale" priority="141">
+    <cfRule type="colorScale" priority="139">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4210,7 +4224,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ6">
-    <cfRule type="colorScale" priority="140">
+    <cfRule type="colorScale" priority="138">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4220,7 +4234,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP7">
-    <cfRule type="colorScale" priority="139">
+    <cfRule type="colorScale" priority="137">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4230,7 +4244,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ2">
-    <cfRule type="colorScale" priority="138">
+    <cfRule type="colorScale" priority="136">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4240,7 +4254,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS2">
-    <cfRule type="colorScale" priority="137">
+    <cfRule type="colorScale" priority="135">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4250,7 +4264,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS3">
-    <cfRule type="colorScale" priority="136">
+    <cfRule type="colorScale" priority="134">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4260,7 +4274,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS4">
-    <cfRule type="colorScale" priority="135">
+    <cfRule type="colorScale" priority="133">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4270,7 +4284,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT2">
-    <cfRule type="colorScale" priority="134">
+    <cfRule type="colorScale" priority="132">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4280,7 +4294,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT3">
-    <cfRule type="colorScale" priority="133">
+    <cfRule type="colorScale" priority="131">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4290,7 +4304,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT4">
-    <cfRule type="colorScale" priority="132">
+    <cfRule type="colorScale" priority="130">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4300,7 +4314,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT5">
-    <cfRule type="colorScale" priority="131">
+    <cfRule type="colorScale" priority="129">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4310,7 +4324,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT6">
-    <cfRule type="colorScale" priority="130">
+    <cfRule type="colorScale" priority="128">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4320,7 +4334,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU4">
-    <cfRule type="colorScale" priority="129">
+    <cfRule type="colorScale" priority="127">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4330,7 +4344,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV3">
-    <cfRule type="colorScale" priority="128">
+    <cfRule type="colorScale" priority="126">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4340,7 +4354,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV5">
-    <cfRule type="colorScale" priority="127">
+    <cfRule type="colorScale" priority="125">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4350,7 +4364,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV6">
-    <cfRule type="colorScale" priority="126">
+    <cfRule type="colorScale" priority="124">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4360,7 +4374,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX2">
-    <cfRule type="colorScale" priority="125">
+    <cfRule type="colorScale" priority="123">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4370,7 +4384,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY2">
-    <cfRule type="colorScale" priority="124">
+    <cfRule type="colorScale" priority="122">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4380,7 +4394,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY3">
-    <cfRule type="colorScale" priority="123">
+    <cfRule type="colorScale" priority="121">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4390,7 +4404,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY4">
-    <cfRule type="colorScale" priority="122">
+    <cfRule type="colorScale" priority="120">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4400,7 +4414,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY5">
-    <cfRule type="colorScale" priority="121">
+    <cfRule type="colorScale" priority="119">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4410,7 +4424,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY6">
-    <cfRule type="colorScale" priority="120">
+    <cfRule type="colorScale" priority="118">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4420,7 +4434,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB6">
-    <cfRule type="colorScale" priority="119">
+    <cfRule type="colorScale" priority="117">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4430,7 +4444,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB5">
-    <cfRule type="colorScale" priority="118">
+    <cfRule type="colorScale" priority="116">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4440,7 +4454,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB4">
-    <cfRule type="colorScale" priority="117">
+    <cfRule type="colorScale" priority="115">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4450,7 +4464,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB3">
-    <cfRule type="colorScale" priority="116">
+    <cfRule type="colorScale" priority="114">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4460,7 +4474,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC3">
-    <cfRule type="colorScale" priority="115">
+    <cfRule type="colorScale" priority="113">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4470,7 +4484,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD3">
-    <cfRule type="colorScale" priority="114">
+    <cfRule type="colorScale" priority="112">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4480,7 +4494,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD4">
-    <cfRule type="colorScale" priority="113">
+    <cfRule type="colorScale" priority="111">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4490,7 +4504,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD5">
-    <cfRule type="colorScale" priority="112">
+    <cfRule type="colorScale" priority="110">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4500,7 +4514,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD6">
-    <cfRule type="colorScale" priority="111">
+    <cfRule type="colorScale" priority="109">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4510,7 +4524,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC4">
-    <cfRule type="colorScale" priority="110">
+    <cfRule type="colorScale" priority="108">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4520,7 +4534,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BF6">
-    <cfRule type="colorScale" priority="109">
+    <cfRule type="colorScale" priority="107">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4530,7 +4544,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BF5">
-    <cfRule type="colorScale" priority="108">
+    <cfRule type="colorScale" priority="106">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4540,7 +4554,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BF4">
-    <cfRule type="colorScale" priority="107">
+    <cfRule type="colorScale" priority="105">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4550,7 +4564,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BF3">
-    <cfRule type="colorScale" priority="106">
+    <cfRule type="colorScale" priority="104">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4560,7 +4574,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG3">
-    <cfRule type="colorScale" priority="105">
+    <cfRule type="colorScale" priority="103">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4570,7 +4584,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BH3">
-    <cfRule type="colorScale" priority="104">
+    <cfRule type="colorScale" priority="102">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4580,7 +4594,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BH4">
-    <cfRule type="colorScale" priority="103">
+    <cfRule type="colorScale" priority="101">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4590,7 +4604,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BH5">
-    <cfRule type="colorScale" priority="102">
+    <cfRule type="colorScale" priority="100">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4600,7 +4614,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BH6">
-    <cfRule type="colorScale" priority="101">
+    <cfRule type="colorScale" priority="99">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4610,7 +4624,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ3">
-    <cfRule type="colorScale" priority="100">
+    <cfRule type="colorScale" priority="98">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4620,7 +4634,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BK3">
-    <cfRule type="colorScale" priority="99">
+    <cfRule type="colorScale" priority="97">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4630,7 +4644,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL3">
-    <cfRule type="colorScale" priority="98">
+    <cfRule type="colorScale" priority="96">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4640,7 +4654,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL4">
-    <cfRule type="colorScale" priority="97">
+    <cfRule type="colorScale" priority="95">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4650,7 +4664,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL5">
-    <cfRule type="colorScale" priority="96">
+    <cfRule type="colorScale" priority="94">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4660,7 +4674,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL6">
-    <cfRule type="colorScale" priority="95">
+    <cfRule type="colorScale" priority="93">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4670,7 +4684,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BK6">
-    <cfRule type="colorScale" priority="94">
+    <cfRule type="colorScale" priority="92">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4680,7 +4694,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ6">
-    <cfRule type="colorScale" priority="93">
+    <cfRule type="colorScale" priority="91">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4690,7 +4704,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ5">
-    <cfRule type="colorScale" priority="92">
+    <cfRule type="colorScale" priority="90">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4700,7 +4714,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ4">
-    <cfRule type="colorScale" priority="91">
+    <cfRule type="colorScale" priority="89">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4710,7 +4724,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BN3">
-    <cfRule type="colorScale" priority="90">
+    <cfRule type="colorScale" priority="88">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4720,7 +4734,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BN4">
-    <cfRule type="colorScale" priority="89">
+    <cfRule type="colorScale" priority="87">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4730,7 +4744,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BN5">
-    <cfRule type="colorScale" priority="88">
+    <cfRule type="colorScale" priority="86">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4740,7 +4754,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BN6">
-    <cfRule type="colorScale" priority="87">
+    <cfRule type="colorScale" priority="85">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4750,7 +4764,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BN7">
-    <cfRule type="colorScale" priority="86">
+    <cfRule type="colorScale" priority="84">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4760,7 +4774,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO6">
-    <cfRule type="colorScale" priority="85">
+    <cfRule type="colorScale" priority="83">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4770,7 +4784,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BP5">
-    <cfRule type="colorScale" priority="84">
+    <cfRule type="colorScale" priority="82">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4780,7 +4794,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BP4">
-    <cfRule type="colorScale" priority="83">
+    <cfRule type="colorScale" priority="81">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4790,7 +4804,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO3">
-    <cfRule type="colorScale" priority="82">
+    <cfRule type="colorScale" priority="80">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4800,7 +4814,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BR4">
-    <cfRule type="colorScale" priority="81">
+    <cfRule type="colorScale" priority="79">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4810,7 +4824,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BR5">
-    <cfRule type="colorScale" priority="80">
+    <cfRule type="colorScale" priority="78">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4820,7 +4834,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BS6">
-    <cfRule type="colorScale" priority="79">
+    <cfRule type="colorScale" priority="77">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4830,7 +4844,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT7">
-    <cfRule type="colorScale" priority="78">
+    <cfRule type="colorScale" priority="76">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4840,7 +4854,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT6">
-    <cfRule type="colorScale" priority="77">
+    <cfRule type="colorScale" priority="75">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4850,7 +4864,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT5">
-    <cfRule type="colorScale" priority="76">
+    <cfRule type="colorScale" priority="74">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4860,7 +4874,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT4">
-    <cfRule type="colorScale" priority="75">
+    <cfRule type="colorScale" priority="73">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4870,7 +4884,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT3">
-    <cfRule type="colorScale" priority="74">
+    <cfRule type="colorScale" priority="72">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4880,7 +4894,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BS3">
-    <cfRule type="colorScale" priority="73">
+    <cfRule type="colorScale" priority="71">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4890,7 +4904,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BV3">
-    <cfRule type="colorScale" priority="72">
+    <cfRule type="colorScale" priority="70">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4900,7 +4914,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BV4">
-    <cfRule type="colorScale" priority="71">
+    <cfRule type="colorScale" priority="69">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4910,7 +4924,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BV5">
-    <cfRule type="colorScale" priority="70">
+    <cfRule type="colorScale" priority="68">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4920,7 +4934,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BV6">
-    <cfRule type="colorScale" priority="69">
+    <cfRule type="colorScale" priority="67">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4930,7 +4944,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BW3">
-    <cfRule type="colorScale" priority="68">
+    <cfRule type="colorScale" priority="66">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4940,7 +4954,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BX3">
-    <cfRule type="colorScale" priority="67">
+    <cfRule type="colorScale" priority="65">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4950,7 +4964,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BX4">
-    <cfRule type="colorScale" priority="66">
+    <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4960,7 +4974,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BZ4">
-    <cfRule type="colorScale" priority="65">
+    <cfRule type="colorScale" priority="63">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4970,7 +4984,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA3">
-    <cfRule type="colorScale" priority="64">
+    <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4980,7 +4994,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CB3">
-    <cfRule type="colorScale" priority="63">
+    <cfRule type="colorScale" priority="61">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4990,7 +5004,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CB5">
-    <cfRule type="colorScale" priority="62">
+    <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5000,7 +5014,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA6">
-    <cfRule type="colorScale" priority="61">
+    <cfRule type="colorScale" priority="59">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5010,7 +5024,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BZ6">
-    <cfRule type="colorScale" priority="60">
+    <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5020,7 +5034,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CD3">
-    <cfRule type="colorScale" priority="59">
+    <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5030,7 +5044,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CF3">
-    <cfRule type="colorScale" priority="57">
+    <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5040,7 +5054,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CE2">
-    <cfRule type="colorScale" priority="56">
+    <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5050,7 +5064,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CE3">
-    <cfRule type="colorScale" priority="55">
+    <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5060,7 +5074,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CE4">
-    <cfRule type="colorScale" priority="54">
+    <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5070,7 +5084,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CE5">
-    <cfRule type="colorScale" priority="53">
+    <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5080,7 +5094,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CF6">
-    <cfRule type="colorScale" priority="52">
+    <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5090,7 +5104,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CH3">
-    <cfRule type="colorScale" priority="51">
+    <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5100,7 +5114,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CH4">
-    <cfRule type="colorScale" priority="50">
+    <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5110,7 +5124,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CH5">
-    <cfRule type="colorScale" priority="49">
+    <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5120,7 +5134,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CH6">
-    <cfRule type="colorScale" priority="48">
+    <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5130,7 +5144,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CI6">
-    <cfRule type="colorScale" priority="47">
+    <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5140,7 +5154,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ6">
-    <cfRule type="colorScale" priority="46">
+    <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5150,7 +5164,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ5">
-    <cfRule type="colorScale" priority="45">
+    <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5160,7 +5174,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ4">
-    <cfRule type="colorScale" priority="44">
+    <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5170,7 +5184,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ3">
-    <cfRule type="colorScale" priority="43">
+    <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5180,7 +5194,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL3">
-    <cfRule type="colorScale" priority="42">
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5190,7 +5204,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL4">
-    <cfRule type="colorScale" priority="41">
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5200,7 +5214,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL5">
-    <cfRule type="colorScale" priority="40">
+    <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5210,7 +5224,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CM6">
-    <cfRule type="colorScale" priority="39">
+    <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5220,7 +5234,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CN5">
-    <cfRule type="colorScale" priority="38">
+    <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5230,7 +5244,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CN4">
-    <cfRule type="colorScale" priority="37">
+    <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5240,7 +5254,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CN3">
-    <cfRule type="colorScale" priority="36">
+    <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5250,7 +5264,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CP3">
-    <cfRule type="colorScale" priority="35">
+    <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5260,7 +5274,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CP4">
-    <cfRule type="colorScale" priority="34">
+    <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5270,7 +5284,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CP5">
-    <cfRule type="colorScale" priority="33">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5280,7 +5294,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CP6">
-    <cfRule type="colorScale" priority="32">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5290,7 +5304,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CQ5">
-    <cfRule type="colorScale" priority="31">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5592,4 +5606,1836 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="2.625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="7">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7">
+        <v>2</v>
+      </c>
+      <c r="E1" s="7">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7">
+        <v>4</v>
+      </c>
+      <c r="G1" s="7">
+        <v>5</v>
+      </c>
+      <c r="H1" s="7">
+        <v>6</v>
+      </c>
+      <c r="I1" s="7">
+        <v>7</v>
+      </c>
+      <c r="J1" s="7">
+        <v>8</v>
+      </c>
+      <c r="K1" s="7">
+        <v>9</v>
+      </c>
+      <c r="L1" s="7">
+        <v>10</v>
+      </c>
+      <c r="M1" s="7">
+        <v>11</v>
+      </c>
+      <c r="N1" s="7">
+        <v>12</v>
+      </c>
+      <c r="O1" s="7">
+        <v>13</v>
+      </c>
+      <c r="P1" s="7">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="7">
+        <v>15</v>
+      </c>
+      <c r="R1" s="7">
+        <v>16</v>
+      </c>
+      <c r="S1" s="7">
+        <v>17</v>
+      </c>
+      <c r="T1" s="7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="T2" s="2"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="T3" s="2"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="2"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M5" s="4"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="2"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>16</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>32</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>64</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>128</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="2" t="str">
+        <f>"0x"&amp;DEC2HEX((SUMIF(C2:C9,"&lt;&gt;",$A2:$A9)),2)&amp;","</f>
+        <v>0x00,</v>
+      </c>
+      <c r="D10" s="2" t="str">
+        <f t="shared" ref="D10:T10" si="0">"0x"&amp;DEC2HEX((SUMIF(D2:D9,"&lt;&gt;",$A2:$A9)),2)&amp;","</f>
+        <v>0x00,</v>
+      </c>
+      <c r="E10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x04,</v>
+      </c>
+      <c r="F10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00,</v>
+      </c>
+      <c r="G10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00,</v>
+      </c>
+      <c r="H10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00,</v>
+      </c>
+      <c r="I10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00,</v>
+      </c>
+      <c r="J10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x02,</v>
+      </c>
+      <c r="K10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00,</v>
+      </c>
+      <c r="L10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x08,</v>
+      </c>
+      <c r="M10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00,</v>
+      </c>
+      <c r="N10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00,</v>
+      </c>
+      <c r="O10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00,</v>
+      </c>
+      <c r="P10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x08,</v>
+      </c>
+      <c r="Q10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00,</v>
+      </c>
+      <c r="R10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x02,</v>
+      </c>
+      <c r="S10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00,</v>
+      </c>
+      <c r="T10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7">
+        <v>1</v>
+      </c>
+      <c r="D12" s="7">
+        <v>2</v>
+      </c>
+      <c r="E12" s="7">
+        <v>3</v>
+      </c>
+      <c r="F12" s="7">
+        <v>4</v>
+      </c>
+      <c r="G12" s="7">
+        <v>5</v>
+      </c>
+      <c r="H12" s="7">
+        <v>6</v>
+      </c>
+      <c r="I12" s="7">
+        <v>7</v>
+      </c>
+      <c r="J12" s="7">
+        <v>8</v>
+      </c>
+      <c r="K12" s="7">
+        <v>9</v>
+      </c>
+      <c r="L12" s="7">
+        <v>10</v>
+      </c>
+      <c r="M12" s="7">
+        <v>11</v>
+      </c>
+      <c r="N12" s="7">
+        <v>12</v>
+      </c>
+      <c r="O12" s="7">
+        <v>13</v>
+      </c>
+      <c r="P12" s="7">
+        <v>14</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>15</v>
+      </c>
+      <c r="R12" s="7">
+        <v>16</v>
+      </c>
+      <c r="S12" s="7">
+        <v>17</v>
+      </c>
+      <c r="T12" s="7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>1</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="T13" s="2"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>2</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2"/>
+      <c r="O14" s="4"/>
+      <c r="Q14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="T14" s="2"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>4</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M15" s="4"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="T15" s="2"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>8</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="4"/>
+      <c r="K16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N16" s="2"/>
+      <c r="O16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S16" s="4"/>
+      <c r="T16" s="2"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="4"/>
+      <c r="K17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N17" s="2"/>
+      <c r="O17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="T17" s="2"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>32</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>64</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>128</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="2" t="str">
+        <f>"0x"&amp;DEC2HEX((SUMIF(C13:C20,"&lt;&gt;",$A13:$A20)),2)&amp;","</f>
+        <v>0x00,</v>
+      </c>
+      <c r="D21" s="2" t="str">
+        <f t="shared" ref="D21" si="1">"0x"&amp;DEC2HEX((SUMIF(D13:D20,"&lt;&gt;",$A13:$A20)),2)&amp;","</f>
+        <v>0x0E,</v>
+      </c>
+      <c r="E21" s="2" t="str">
+        <f t="shared" ref="E21" si="2">"0x"&amp;DEC2HEX((SUMIF(E13:E20,"&lt;&gt;",$A13:$A20)),2)&amp;","</f>
+        <v>0x0E,</v>
+      </c>
+      <c r="F21" s="2" t="str">
+        <f t="shared" ref="F21" si="3">"0x"&amp;DEC2HEX((SUMIF(F13:F20,"&lt;&gt;",$A13:$A20)),2)&amp;","</f>
+        <v>0x0E,</v>
+      </c>
+      <c r="G21" s="2" t="str">
+        <f t="shared" ref="G21" si="4">"0x"&amp;DEC2HEX((SUMIF(G13:G20,"&lt;&gt;",$A13:$A20)),2)&amp;","</f>
+        <v>0x00,</v>
+      </c>
+      <c r="H21" s="2" t="str">
+        <f t="shared" ref="H21" si="5">"0x"&amp;DEC2HEX((SUMIF(H13:H20,"&lt;&gt;",$A13:$A20)),2)&amp;","</f>
+        <v>0x00,</v>
+      </c>
+      <c r="I21" s="2" t="str">
+        <f t="shared" ref="I21" si="6">"0x"&amp;DEC2HEX((SUMIF(I13:I20,"&lt;&gt;",$A13:$A20)),2)&amp;","</f>
+        <v>0x07,</v>
+      </c>
+      <c r="J21" s="2" t="str">
+        <f t="shared" ref="J21" si="7">"0x"&amp;DEC2HEX((SUMIF(J13:J20,"&lt;&gt;",$A13:$A20)),2)&amp;","</f>
+        <v>0x07,</v>
+      </c>
+      <c r="K21" s="2" t="str">
+        <f t="shared" ref="K21" si="8">"0x"&amp;DEC2HEX((SUMIF(K13:K20,"&lt;&gt;",$A13:$A20)),2)&amp;","</f>
+        <v>0x1F,</v>
+      </c>
+      <c r="L21" s="2" t="str">
+        <f t="shared" ref="L21" si="9">"0x"&amp;DEC2HEX((SUMIF(L13:L20,"&lt;&gt;",$A13:$A20)),2)&amp;","</f>
+        <v>0x1C,</v>
+      </c>
+      <c r="M21" s="2" t="str">
+        <f t="shared" ref="M21" si="10">"0x"&amp;DEC2HEX((SUMIF(M13:M20,"&lt;&gt;",$A13:$A20)),2)&amp;","</f>
+        <v>0x18,</v>
+      </c>
+      <c r="N21" s="2" t="str">
+        <f t="shared" ref="N21" si="11">"0x"&amp;DEC2HEX((SUMIF(N13:N20,"&lt;&gt;",$A13:$A20)),2)&amp;","</f>
+        <v>0x00,</v>
+      </c>
+      <c r="O21" s="2" t="str">
+        <f t="shared" ref="O21" si="12">"0x"&amp;DEC2HEX((SUMIF(O13:O20,"&lt;&gt;",$A13:$A20)),2)&amp;","</f>
+        <v>0x1C,</v>
+      </c>
+      <c r="P21" s="2" t="str">
+        <f t="shared" ref="P21" si="13">"0x"&amp;DEC2HEX((SUMIF(P13:P20,"&lt;&gt;",$A13:$A20)),2)&amp;","</f>
+        <v>0x1C,</v>
+      </c>
+      <c r="Q21" s="2" t="str">
+        <f t="shared" ref="Q21" si="14">"0x"&amp;DEC2HEX((SUMIF(Q13:Q20,"&lt;&gt;",$A13:$A20)),2)&amp;","</f>
+        <v>0x1F,</v>
+      </c>
+      <c r="R21" s="2" t="str">
+        <f t="shared" ref="R21" si="15">"0x"&amp;DEC2HEX((SUMIF(R13:R20,"&lt;&gt;",$A13:$A20)),2)&amp;","</f>
+        <v>0x07,</v>
+      </c>
+      <c r="S21" s="2" t="str">
+        <f t="shared" ref="S21" si="16">"0x"&amp;DEC2HEX((SUMIF(S13:S20,"&lt;&gt;",$A13:$A20)),2)&amp;","</f>
+        <v>0x07,</v>
+      </c>
+      <c r="T21" s="2" t="str">
+        <f t="shared" ref="T21" si="17">"0x"&amp;DEC2HEX((SUMIF(T13:T20,"&lt;&gt;",$A13:$A20)),2)&amp;","</f>
+        <v>0x00,</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C24" s="1" t="str">
+        <f>_xlfn.CONCAT(C10,C21)</f>
+        <v>0x00,0x00,</v>
+      </c>
+      <c r="D24" s="1" t="str">
+        <f t="shared" ref="D24:T24" si="18">_xlfn.CONCAT(D10,D21)</f>
+        <v>0x00,0x0E,</v>
+      </c>
+      <c r="E24" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>0x04,0x0E,</v>
+      </c>
+      <c r="F24" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>0x00,0x0E,</v>
+      </c>
+      <c r="G24" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>0x00,0x00,</v>
+      </c>
+      <c r="I24" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>0x00,0x07,</v>
+      </c>
+      <c r="J24" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>0x02,0x07,</v>
+      </c>
+      <c r="K24" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>0x00,0x1F,</v>
+      </c>
+      <c r="L24" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>0x08,0x1C,</v>
+      </c>
+      <c r="M24" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>0x00,0x18,</v>
+      </c>
+      <c r="O24" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>0x00,0x1C,</v>
+      </c>
+      <c r="P24" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>0x08,0x1C,</v>
+      </c>
+      <c r="Q24" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>0x00,0x1F,</v>
+      </c>
+      <c r="R24" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>0x02,0x07,</v>
+      </c>
+      <c r="S24" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>0x00,0x07,</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="colorScale" priority="382">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3">
+    <cfRule type="colorScale" priority="381">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4">
+    <cfRule type="colorScale" priority="380">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5">
+    <cfRule type="colorScale" priority="379">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="colorScale" priority="378">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="colorScale" priority="377">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="colorScale" priority="376">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="colorScale" priority="375">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="colorScale" priority="374">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="colorScale" priority="373">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="colorScale" priority="372">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="colorScale" priority="371">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4">
+    <cfRule type="colorScale" priority="370">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5">
+    <cfRule type="colorScale" priority="369">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="colorScale" priority="144">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="colorScale" priority="143">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4">
+    <cfRule type="colorScale" priority="142">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="colorScale" priority="141">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6">
+    <cfRule type="colorScale" priority="140">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2">
+    <cfRule type="colorScale" priority="139">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2">
+    <cfRule type="colorScale" priority="138">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3">
+    <cfRule type="colorScale" priority="137">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4">
+    <cfRule type="colorScale" priority="136">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5">
+    <cfRule type="colorScale" priority="135">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K6">
+    <cfRule type="colorScale" priority="134">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J4">
+    <cfRule type="colorScale" priority="133">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M4">
+    <cfRule type="colorScale" priority="132">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M5">
+    <cfRule type="colorScale" priority="131">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2">
+    <cfRule type="colorScale" priority="130">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O3">
+    <cfRule type="colorScale" priority="129">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O4">
+    <cfRule type="colorScale" priority="128">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O5">
+    <cfRule type="colorScale" priority="127">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O6">
+    <cfRule type="colorScale" priority="126">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2">
+    <cfRule type="colorScale" priority="125">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q2">
+    <cfRule type="colorScale" priority="124">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q3">
+    <cfRule type="colorScale" priority="123">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q4">
+    <cfRule type="colorScale" priority="122">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q5">
+    <cfRule type="colorScale" priority="121">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q6">
+    <cfRule type="colorScale" priority="120">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P4">
+    <cfRule type="colorScale" priority="119">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S4">
+    <cfRule type="colorScale" priority="118">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S5">
+    <cfRule type="colorScale" priority="117">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3">
+    <cfRule type="colorScale" priority="88">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L5">
+    <cfRule type="colorScale" priority="87">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P5">
+    <cfRule type="colorScale" priority="86">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R3">
+    <cfRule type="colorScale" priority="85">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="colorScale" priority="84">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="colorScale" priority="83">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="colorScale" priority="82">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="colorScale" priority="81">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17">
+    <cfRule type="colorScale" priority="80">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="colorScale" priority="79">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="colorScale" priority="78">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="colorScale" priority="76">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17">
+    <cfRule type="colorScale" priority="74">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G15">
+    <cfRule type="colorScale" priority="72">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G16">
+    <cfRule type="colorScale" priority="71">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
+    <cfRule type="colorScale" priority="67">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
+    <cfRule type="colorScale" priority="66">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M15">
+    <cfRule type="colorScale" priority="58">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O13">
+    <cfRule type="colorScale" priority="56">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O14">
+    <cfRule type="colorScale" priority="55">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P13">
+    <cfRule type="colorScale" priority="51">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S16">
+    <cfRule type="colorScale" priority="43">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J14">
+    <cfRule type="colorScale" priority="42">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L16">
+    <cfRule type="colorScale" priority="41">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P16">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K14">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K13">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J13">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L17">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M17">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M16">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L15">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O15">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P15">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q15">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R15">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S15">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S14">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R14">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q14">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q13">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R13">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S13">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q16">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O16">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O17">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P17">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>